<commit_message>
added OnEachRow test when using WithGroupedHeaders
</commit_message>
<xml_diff>
--- a/tests/Data/Disks/Local/import-users-with-grouped-headers.xlsx
+++ b/tests/Data/Disks/Local/import-users-with-grouped-headers.xlsx
@@ -5,17 +5,17 @@
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vendorfuel\Apps\forked-excel\tests\Data\Disks\Local\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vendorfuel\Apps\laravel-excel-public\tests\Data\Disks\Local\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7EB2D5-746D-4027-B69A-CA104AA53CE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62CDEA0-2BD8-4065-8F85-645169927292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6195" yWindow="2325" windowWidth="17520" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3975" yWindow="2235" windowWidth="14595" windowHeight="11865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,18 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>patrick@maatwebsite.nl</t>
   </si>
   <si>
-    <t>taylor@laravel.com</t>
-  </si>
-  <si>
     <t>Patrick Brouwers</t>
-  </si>
-  <si>
-    <t>Taylor Otwell</t>
   </si>
   <si>
     <t>name</t>
@@ -400,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,51 +408,36 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{20A9DBB9-44E1-4501-BEC8-518F447F4B24}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>